<commit_message>
Reworked initial set of functions
</commit_message>
<xml_diff>
--- a/inst/models/oxygen.xlsx
+++ b/inst/models/oxygen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -34,10 +34,7 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">value.default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value.alternative</t>
+    <t xml:space="preserve">default</t>
   </si>
   <si>
     <t xml:space="preserve">OM</t>
@@ -309,13 +306,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.67"/>
   </cols>
@@ -333,41 +330,32 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -387,13 +375,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -408,75 +396,60 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>10</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2.67</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>2.67</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -502,7 +475,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -517,13 +490,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -544,11 +517,11 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.13"/>
@@ -566,47 +539,47 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>-1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>0</v>

</xml_diff>